<commit_message>
barranco alto, grant amount.
</commit_message>
<xml_diff>
--- a/RCLA_Projects_Formatted.xlsx
+++ b/RCLA_Projects_Formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mrosen\rcla_project_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198D14BC-944A-40FA-B2CB-A7D58CFF5507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C918B816-84D4-4A86-836A-555DBFC867CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-66950" yWindow="-3100" windowWidth="25090" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-66500" yWindow="-2650" windowWidth="25090" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCLA_Projects" sheetId="1" r:id="rId1"/>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1547,6 +1547,9 @@
       <c r="G12" t="s">
         <v>75</v>
       </c>
+      <c r="H12">
+        <v>9580</v>
+      </c>
       <c r="I12" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
support proposed projects, update prior to Calgary show.
</commit_message>
<xml_diff>
--- a/RCLA_Projects_Formatted.xlsx
+++ b/RCLA_Projects_Formatted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\msr\rcla_project_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18EE66C-C15B-4A67-955F-A585B51F7FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6BDD1FF-B124-4661-ABE3-F7EEB984A2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -343,6 +343,51 @@
   </si>
   <si>
     <t>GG2570080</t>
+  </si>
+  <si>
+    <t>GG2574529</t>
+  </si>
+  <si>
+    <t>Reforesting Santiago</t>
+  </si>
+  <si>
+    <t>proposed</t>
+  </si>
+  <si>
+    <t>This project restores ecosystems, provides families with sustainable source of firewood, imporoves access to clean water and strengthens community resilience.</t>
+  </si>
+  <si>
+    <t>Rotary E-Club San Diego Global</t>
+  </si>
+  <si>
+    <t>WKG</t>
+  </si>
+  <si>
+    <t>ADP_VistaHermosa</t>
+  </si>
+  <si>
+    <t>ADP_Panimaquip</t>
+  </si>
+  <si>
+    <t>Water and Sanitation for Panimaquip, San Lucas Toliman</t>
+  </si>
+  <si>
+    <t>Sanitation for Vista Hermosa, Santa Lucia Utatlan</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1piFpvjaRl6BletKqpdrz2wlrc7pAYXgqHn6leAGrNto/edit?tab=t.0</t>
+  </si>
+  <si>
+    <t>This project povides sanitation services for 30 familes.  This is a follow-on project to an earlier grant that rehabiliated a potable water system.</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1DhmMi5CsALaOjiPloV8raZ8VPry1vaK8zJoh0PWGvdo/edit?tab=t.0</t>
+  </si>
+  <si>
+    <t>This project rehabiltates a potable water system.</t>
+  </si>
+  <si>
+    <t>Bruce</t>
   </si>
 </sst>
 </file>
@@ -477,6 +522,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}" name="Table1" displayName="Table1" ref="A1:M19" totalsRowShown="0">
+  <autoFilter ref="A1:M19" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{968E55D8-D786-4B51-912C-1987D80112F4}" name="id"/>
+    <tableColumn id="2" xr3:uid="{8B850DEB-CA89-491D-B41E-53DEB8A95556}" name="position_lat"/>
+    <tableColumn id="3" xr3:uid="{37CCEF96-76CA-4794-A355-391672288D98}" name="position_lng"/>
+    <tableColumn id="4" xr3:uid="{4EB3EB66-FA8D-40BA-9ADF-37979D4C550A}" name="url"/>
+    <tableColumn id="5" xr3:uid="{76F97B48-C72D-4B56-94CD-5FE9425CD805}" name="title"/>
+    <tableColumn id="6" xr3:uid="{81B1D5C7-B572-45FF-BB60-6F4EE0820CA7}" name="status"/>
+    <tableColumn id="7" xr3:uid="{2236368A-6625-4649-8B21-D00A31D0117A}" name="shepard"/>
+    <tableColumn id="8" xr3:uid="{E5A0B68B-E6FB-46C2-82F6-0362F4EEF036}" name="description"/>
+    <tableColumn id="9" xr3:uid="{E744ADBA-83A3-49C0-BF6C-678034A6ACBD}" name="grantAmount"/>
+    <tableColumn id="10" xr3:uid="{A1EB0F2C-8CCD-4336-A31B-3F46432D7085}" name="internationalClub_name"/>
+    <tableColumn id="11" xr3:uid="{8FFD48CF-3AE8-49F2-AF28-F6278B055668}" name="internationalClub_district"/>
+    <tableColumn id="12" xr3:uid="{037FF40C-65F6-45A1-9A54-90B273B5BCBF}" name="partner"/>
+    <tableColumn id="13" xr3:uid="{7CADDF70-1EC9-4474-813D-5BC536A83823}" name="period"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,17 +722,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M1048574"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="59.1796875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
@@ -673,7 +740,7 @@
     <col min="8" max="8" width="30.6328125" customWidth="1"/>
     <col min="9" max="9" width="24.453125" customWidth="1"/>
     <col min="10" max="10" width="23.7265625" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" customWidth="1"/>
+    <col min="11" max="11" width="24.54296875" customWidth="1"/>
     <col min="12" max="12" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,7 +913,7 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -1282,13 +1349,124 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="1048575" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17">
+        <v>14.600127799999999</v>
+      </c>
+      <c r="C17">
+        <v>-91.226982599999999</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17">
+        <v>38000</v>
+      </c>
+      <c r="J17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>5340</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18">
+        <v>14.777010000000001</v>
+      </c>
+      <c r="C18">
+        <v>-91.267499999999998</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18">
+        <v>50000</v>
+      </c>
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19">
+        <v>14.600020000000001</v>
+      </c>
+      <c r="C19">
+        <v>-91.147509999999997</v>
+      </c>
+      <c r="D19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19">
+        <v>50000</v>
+      </c>
+      <c r="L19" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D11" r:id="rId1" display="https://www.facebook.com/permalink.php?story_fbid=pfbid02tNeGRHDMdBffMFukX571gYoddb77PD9kZ9TadKkXEiJpS1hSzkN7X27S6T6KNaMMl&amp;id=100064244756826&amp;__cft__[0]=AZXqZ5WH0GRdeeI7s7vPTWfYaGzfZCUg5OxfnPn1esLvvnGwkt34FjlQZTX5eXEd4qJnZAW99AhzixUvtdHedujyR6pv1Ux3jm9L2VtAPTRMkFKHsr0Z9pUke2XOb1IkOBMmEtOXHkhQPOUYrSsJ3__8HUfeAIrCfqaJlrh_LN58BEv9StI3aM2lhj6lwmzfplY&amp;__tn__=%2CO%2CP-R" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
closed s.c.1, approved Hospitalito and Reforestation.
</commit_message>
<xml_diff>
--- a/RCLA_Projects_Formatted.xlsx
+++ b/RCLA_Projects_Formatted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\msr\rcla_project_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6BDD1FF-B124-4661-ABE3-F7EEB984A2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E34978E-6FE1-46AD-B952-7C0882E1A9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -388,6 +388,12 @@
   </si>
   <si>
     <t>Bruce</t>
+  </si>
+  <si>
+    <t>https://rotaryatitlan.org/hospitalito-grant-2025/</t>
+  </si>
+  <si>
+    <t>https://rotaryatitlan.org/visiting-our-friends-amigos-de-santa-cruz/</t>
   </si>
 </sst>
 </file>
@@ -724,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1048574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,11 +874,14 @@
       <c r="C4">
         <v>-91.2042</v>
       </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
       <c r="E4" t="s">
         <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>27</v>
@@ -1245,6 +1254,9 @@
       <c r="C14">
         <v>-91.204300000000003</v>
       </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
       <c r="E14" t="s">
         <v>88</v>
       </c>
@@ -1283,6 +1295,9 @@
       <c r="C15">
         <v>-91.204400000000007</v>
       </c>
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
       <c r="E15" t="s">
         <v>89</v>
       </c>
@@ -1321,6 +1336,9 @@
       <c r="C16">
         <v>-91.2247603881152</v>
       </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
       <c r="E16" t="s">
         <v>90</v>
       </c>
@@ -1363,7 +1381,7 @@
         <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
update data source; https for icon fetches and other clean up
</commit_message>
<xml_diff>
--- a/RCLA_Projects_Formatted.xlsx
+++ b/RCLA_Projects_Formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\msr\rcla_project_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E34978E-6FE1-46AD-B952-7C0882E1A9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CD810E-5F53-414F-A50F-9C41CAEC75C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="230" yWindow="2660" windowWidth="25370" windowHeight="7980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCLA_Projects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
   <si>
     <t>id</t>
   </si>
@@ -130,11 +130,6 @@
   </si>
   <si>
     <t xml:space="preserve">Joe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The two villages we will be working in are Chuitzam, Santa Lucía Utatlan (population 682) and Chuti Estancia,
-San Andreas Semetabaj (population 1520). Both of these villages have a sever potable water shortage and they
-have to walk a long distance to carry water at this time. </t>
   </si>
   <si>
     <t>Northfield, MN</t>
@@ -363,24 +358,15 @@
     <t>WKG</t>
   </si>
   <si>
-    <t>ADP_VistaHermosa</t>
-  </si>
-  <si>
     <t>ADP_Panimaquip</t>
   </si>
   <si>
     <t>Water and Sanitation for Panimaquip, San Lucas Toliman</t>
   </si>
   <si>
-    <t>Sanitation for Vista Hermosa, Santa Lucia Utatlan</t>
-  </si>
-  <si>
     <t>https://docs.google.com/document/d/1piFpvjaRl6BletKqpdrz2wlrc7pAYXgqHn6leAGrNto/edit?tab=t.0</t>
   </si>
   <si>
-    <t>This project povides sanitation services for 30 familes.  This is a follow-on project to an earlier grant that rehabiliated a potable water system.</t>
-  </si>
-  <si>
     <t>https://docs.google.com/document/d/1DhmMi5CsALaOjiPloV8raZ8VPry1vaK8zJoh0PWGvdo/edit?tab=t.0</t>
   </si>
   <si>
@@ -394,13 +380,128 @@
   </si>
   <si>
     <t>https://rotaryatitlan.org/visiting-our-friends-amigos-de-santa-cruz/</t>
+  </si>
+  <si>
+    <t>GG2684872</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>WKG, Water4Life</t>
+  </si>
+  <si>
+    <t>This project will provide clean drinking water through household filters and sanitation systems while restoring degraded hillsides through the planting of thousands of native trees. The project also includes environmental education to promote long-term stewardship of water and natural resources. Together, these efforts aim to improve public health, reduce water contamination, and protect the watershed for future generations.</t>
+  </si>
+  <si>
+    <t>GG2570516</t>
+  </si>
+  <si>
+    <t>Water, Sanitation, Hygiene for Vista Hermosa, Phase I</t>
+  </si>
+  <si>
+    <t>Clint</t>
+  </si>
+  <si>
+    <t>Annapolis</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The project will deliver a new well, pump, and household water distribution system to provide reliable potable water to families and a school in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Vista Hermosa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> near </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Santa Lucía Utatlán</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Guatemala</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>GG2684482</t>
+  </si>
+  <si>
+    <t>Agroecological Vegetable Production in Santa Cruz La Laguna</t>
+  </si>
+  <si>
+    <t>Mildmay, Ontario Canada</t>
+  </si>
+  <si>
+    <t>AdSC</t>
+  </si>
+  <si>
+    <t>The project promotes sustainable economic development through agroecological vegetable production and commercialization in Santa Cruz La Laguna, Guatemala, focusing on highly vulnerable upper communities such as Chuitzanchaj.  It provides training in business management, collective organization, productivity, post-harvest processing, and the creation of a local market to improve incomes and nutrition.  The project directly benefits 15 indigenous farming families (prioritizing women) and indirectly supports about 850 community members</t>
+  </si>
+  <si>
+    <t>Protecting the Watershed of Lake Atitlan, Santa Lucia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two villages we will be working in are Chuitzam, Santa Lucía Utatlan (population 682) and Chuti Estancia,
+San Andreas Semetabaj (population 1520). Both of these villages have a severe potable water shortage and they
+have to walk a long distance to carry water at this time. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +513,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -531,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}" name="Table1" displayName="Table1" ref="A1:M19" totalsRowShown="0">
-  <autoFilter ref="A1:M19" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}" name="Table1" displayName="Table1" ref="A1:M23" totalsRowShown="0">
+  <autoFilter ref="A1:M23" xr:uid="{AF9BC86D-7ABE-40FD-82C2-07D851E6AD12}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{968E55D8-D786-4B51-912C-1987D80112F4}" name="id"/>
     <tableColumn id="2" xr3:uid="{8B850DEB-CA89-491D-B41E-53DEB8A95556}" name="position_lat"/>
@@ -730,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1048574"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -875,10 +984,10 @@
         <v>-91.2042</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -928,19 +1037,19 @@
         <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="I5">
         <v>161100</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5">
         <v>5960</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5">
         <v>2020</v>
@@ -948,7 +1057,7 @@
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>14.72823</v>
@@ -957,22 +1066,22 @@
         <v>-91.075400000000002</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="I6" s="1">
         <v>50342</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="1">
         <v>5440</v>
@@ -981,12 +1090,12 @@
         <v>25</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>14.63551</v>
@@ -995,7 +1104,7 @@
         <v>-91.14264</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -1004,13 +1113,13 @@
         <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7">
         <v>55823</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7">
         <v>5960</v>
@@ -1019,12 +1128,12 @@
         <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>14.7544</v>
@@ -1033,19 +1142,19 @@
         <v>-90.989829999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8">
         <v>95600</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K8">
         <v>5960</v>
@@ -1056,7 +1165,7 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>14.639426</v>
@@ -1065,19 +1174,19 @@
         <v>-91.218237999999999</v>
       </c>
       <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
         <v>53</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
         <v>55</v>
-      </c>
-      <c r="H9" t="s">
-        <v>56</v>
       </c>
       <c r="L9" t="s">
         <v>25</v>
@@ -1088,7 +1197,7 @@
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <v>14.620979999999999</v>
@@ -1097,10 +1206,10 @@
         <v>-91.238140000000001</v>
       </c>
       <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1109,13 +1218,13 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10">
         <v>117839</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10">
         <v>7670</v>
@@ -1124,12 +1233,12 @@
         <v>25</v>
       </c>
       <c r="M10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>14.7446660257835</v>
@@ -1138,25 +1247,25 @@
         <v>-91.123643530897894</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
         <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
         <v>66</v>
-      </c>
-      <c r="H11" t="s">
-        <v>67</v>
       </c>
       <c r="I11">
         <v>9580</v>
       </c>
       <c r="J11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11">
         <v>2992</v>
@@ -1167,7 +1276,7 @@
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>14.635115984513201</v>
@@ -1176,36 +1285,36 @@
         <v>-91.152687217249095</v>
       </c>
       <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
         <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12">
         <v>89577</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K12">
         <v>5170</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13">
         <v>14.765494074359999</v>
@@ -1214,10 +1323,10 @@
         <v>-91.126203096043199</v>
       </c>
       <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
         <v>76</v>
-      </c>
-      <c r="E13" t="s">
-        <v>77</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1226,27 +1335,27 @@
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I13">
         <v>3000</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K13">
         <v>5240</v>
       </c>
       <c r="L13" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" t="s">
         <v>80</v>
-      </c>
-      <c r="M13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14">
         <v>14.742190000000001</v>
@@ -1255,10 +1364,10 @@
         <v>-91.204300000000003</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
         <v>21</v>
@@ -1267,7 +1376,7 @@
         <v>27</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I14">
         <v>39980</v>
@@ -1279,7 +1388,7 @@
         <v>6330</v>
       </c>
       <c r="L14" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="M14">
         <v>2024</v>
@@ -1287,7 +1396,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>14.742190000000001</v>
@@ -1296,10 +1405,10 @@
         <v>-91.204400000000007</v>
       </c>
       <c r="D15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
@@ -1308,19 +1417,19 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I15">
         <v>55000</v>
       </c>
       <c r="J15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K15">
         <v>6330</v>
       </c>
       <c r="L15" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="M15">
         <v>2024</v>
@@ -1328,7 +1437,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16">
         <v>14.650023791634</v>
@@ -1337,31 +1446,31 @@
         <v>-91.2247603881152</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
       <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
         <v>91</v>
-      </c>
-      <c r="H16" t="s">
-        <v>92</v>
       </c>
       <c r="I16">
         <v>136000</v>
       </c>
       <c r="J16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K16">
         <v>5190</v>
       </c>
       <c r="L16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M16">
         <v>2025</v>
@@ -1369,7 +1478,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17">
         <v>14.600127799999999</v>
@@ -1378,28 +1487,28 @@
         <v>-91.226982599999999</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I17">
         <v>38000</v>
       </c>
       <c r="J17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17">
         <v>5340</v>
       </c>
       <c r="L17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M17">
         <v>2025</v>
@@ -1407,7 +1516,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B18">
         <v>14.777010000000001</v>
@@ -1416,25 +1525,31 @@
         <v>-91.267499999999998</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="I18">
-        <v>50000</v>
+        <v>34140</v>
+      </c>
+      <c r="J18" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18">
+        <v>7620</v>
       </c>
       <c r="L18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M18">
         <v>2025</v>
@@ -1442,7 +1557,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B19">
         <v>14.600020000000001</v>
@@ -1451,27 +1566,103 @@
         <v>-91.147509999999997</v>
       </c>
       <c r="D19" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H19" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I19">
         <v>50000</v>
       </c>
       <c r="L19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M19">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20">
+        <v>14.7687463163484</v>
+      </c>
+      <c r="C20">
+        <v>-91.266137294845507</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20">
+        <v>38800</v>
+      </c>
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20">
+        <v>6330</v>
+      </c>
+      <c r="L20" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21">
+        <v>14.739000000000001</v>
+      </c>
+      <c r="C21">
+        <v>-91.213999999999999</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21">
+        <v>45000</v>
+      </c>
+      <c r="J21" t="s">
+        <v>120</v>
+      </c>
+      <c r="K21">
+        <v>6330</v>
+      </c>
+      <c r="L21" t="s">
+        <v>121</v>
+      </c>
+      <c r="M21">
         <v>2025</v>
       </c>
     </row>

</xml_diff>